<commit_message>
Finished lab2, started lab3
</commit_message>
<xml_diff>
--- a/Zad2/times.xlsx
+++ b/Zad2/times.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\szynt\Desktop\Programming_Playground\University\Algorytmy_Geometryczne\Zad2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90B95DBC-B1AC-44EF-8BA4-63EB3DC52CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF4BA985-CAE5-49B5-AD93-2A4FD6791898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -112,7 +112,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.00,E+00&quot; [s]&quot;"/>
+    <numFmt numFmtId="164" formatCode="0.00E+00&quot; [s]&quot;"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -301,31 +301,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -644,8 +643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8104C01-268E-4912-B9E8-B1E46C5E585E}">
   <dimension ref="A1:AC28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" topLeftCell="D10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26:F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -670,70 +669,70 @@
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
         <v>3.3954143524169903E-4</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="3"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="2"/>
       <c r="L3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
         <v>6.3792943954467699E-4</v>
       </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="6"/>
-      <c r="L4" s="10" t="s">
+      <c r="G4" s="4"/>
+      <c r="H4" s="5"/>
+      <c r="L4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="9" t="s">
+      <c r="M4" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5">
         <v>2.8869152069091702E-4</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="3"/>
-      <c r="K5" s="8" t="s">
+      <c r="G5" s="1"/>
+      <c r="H5" s="2"/>
+      <c r="K5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="L5" s="13">
+      <c r="L5" s="12">
         <v>3.3954143524169903E-4</v>
       </c>
-      <c r="M5" s="14">
+      <c r="M5" s="13">
         <v>6.3792943954467699E-4</v>
       </c>
       <c r="N5" t="b">
@@ -742,24 +741,24 @@
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6">
         <v>1.11423826217651E-2</v>
       </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="6"/>
-      <c r="K6" s="9" t="s">
+      <c r="G6" s="4"/>
+      <c r="H6" s="5"/>
+      <c r="K6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="15">
+      <c r="L6" s="14">
         <v>2.8869152069091702E-4</v>
       </c>
-      <c r="M6" s="16">
+      <c r="M6" s="15">
         <v>1.11423826217651E-2</v>
       </c>
       <c r="N6" t="b">
@@ -768,24 +767,24 @@
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7">
         <v>1.1262130737304599E-3</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="3"/>
-      <c r="K7" s="8" t="s">
+      <c r="G7" s="1"/>
+      <c r="H7" s="2"/>
+      <c r="K7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L7" s="17">
+      <c r="L7" s="16">
         <v>1.1262130737304599E-3</v>
       </c>
-      <c r="M7" s="18">
+      <c r="M7" s="17">
         <v>2.89027690887451E-4</v>
       </c>
       <c r="N7" t="b">
@@ -794,24 +793,24 @@
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8">
         <v>1.2259864807128899E-3</v>
       </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="6"/>
-      <c r="K8" s="9" t="s">
+      <c r="G8" s="4"/>
+      <c r="H8" s="5"/>
+      <c r="K8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L8" s="19">
+      <c r="L8" s="18">
         <v>7.7739715576171796E-4</v>
       </c>
-      <c r="M8" s="20">
+      <c r="M8" s="19">
         <v>1.2259864807128899E-3</v>
       </c>
       <c r="N8" t="b">
@@ -820,98 +819,98 @@
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="1" t="s">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9">
         <v>7.7739715576171796E-4</v>
       </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="3"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="1" t="s">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10">
         <v>2.89027690887451E-4</v>
       </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="6"/>
-      <c r="L10" s="12"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="5"/>
+      <c r="L10" s="11"/>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>4</v>
       </c>
-      <c r="L11" s="11" t="s">
+      <c r="L11" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="1" t="s">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12">
         <v>3.5951137542724601E-4</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H12" s="3" t="s">
+      <c r="G12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="3">
         <v>4.7444510459899898E-3</v>
       </c>
-      <c r="L12" s="10" t="s">
+      <c r="L12" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="M12" s="9" t="s">
+      <c r="M12" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="1" t="s">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13">
         <v>6.4768552780151295E-4</v>
       </c>
-      <c r="G13" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H13" s="6" t="s">
+      <c r="G13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I13" s="7">
+      <c r="I13" s="6">
         <v>7.7062821388244598E-3</v>
       </c>
-      <c r="K13" s="8" t="s">
+      <c r="K13" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="L13" s="18">
+      <c r="L13" s="17">
         <v>3.5951137542724601E-4</v>
       </c>
-      <c r="M13" s="21">
+      <c r="M13" s="20">
         <v>6.4768552780151295E-4</v>
       </c>
       <c r="N13" t="b">
@@ -920,31 +919,31 @@
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="1" t="s">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14">
         <v>1.3952732086181601E-4</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H14" s="3" t="s">
+      <c r="G14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I14" s="3">
         <v>4.3047237396240199E-3</v>
       </c>
-      <c r="K14" s="9" t="s">
+      <c r="K14" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="L14" s="22">
+      <c r="L14" s="21">
         <v>1.3952732086181601E-4</v>
       </c>
-      <c r="M14" s="15">
+      <c r="M14" s="14">
         <v>1.1368823051452601E-3</v>
       </c>
       <c r="N14" t="b">
@@ -953,31 +952,31 @@
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="1" t="s">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15">
         <v>1.1368823051452601E-3</v>
       </c>
-      <c r="G15" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H15" s="6" t="s">
+      <c r="G15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I15" s="7">
+      <c r="I15" s="6">
         <v>0.58616441011428799</v>
       </c>
-      <c r="K15" s="8" t="s">
+      <c r="K15" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L15" s="18">
+      <c r="L15" s="17">
         <v>3.7887334823608298E-4</v>
       </c>
-      <c r="M15" s="23" t="s">
+      <c r="M15" s="22" t="s">
         <v>18</v>
       </c>
       <c r="N15" t="b">
@@ -989,31 +988,31 @@
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="1" t="s">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16">
         <v>3.7887334823608298E-4</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H16" s="3" t="s">
+      <c r="G16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I16" s="4">
+      <c r="I16" s="3">
         <v>6.5287613868713302E-3</v>
       </c>
-      <c r="K16" s="9" t="s">
+      <c r="K16" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L16" s="22">
+      <c r="L16" s="21">
         <v>5.6739807128906199E-4</v>
       </c>
-      <c r="M16" s="15">
+      <c r="M16" s="14">
         <v>2.4915933609008701E-4</v>
       </c>
       <c r="N16" t="b">
@@ -1022,102 +1021,102 @@
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="1" t="s">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17">
         <v>1.2986326217651299E-2</v>
       </c>
-      <c r="G17" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H17" s="6" t="s">
+      <c r="G17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H17" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I17" s="7">
+      <c r="I17" s="6">
         <v>5.3519296646118101E-3</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" s="1" t="s">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18">
         <v>5.6739807128906199E-4</v>
       </c>
-      <c r="G18" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H18" s="3" t="s">
+      <c r="G18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I18" s="4">
+      <c r="I18" s="3">
         <v>8.9594340324401795E-3</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="1" t="s">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19">
         <v>2.4915933609008701E-4</v>
       </c>
-      <c r="G19" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H19" s="6" t="s">
+      <c r="G19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I19" s="7">
+      <c r="I19" s="6">
         <v>2.5084996223449698E-3</v>
       </c>
-      <c r="L19" s="11" t="s">
+      <c r="L19" s="10" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
+      <c r="A20" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" t="s">
         <v>4</v>
       </c>
-      <c r="L20" s="10" t="s">
+      <c r="L20" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="M20" s="9" t="s">
+      <c r="M20" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" s="1" t="s">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21">
         <v>4.7444510459899898E-3</v>
       </c>
-      <c r="K21" s="8" t="s">
+      <c r="K21" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="L21" s="21">
+      <c r="L21" s="20">
         <v>4.7444510459899898E-3</v>
       </c>
-      <c r="M21" s="18">
+      <c r="M21" s="17">
         <v>7.7062821388244598E-3</v>
       </c>
       <c r="N21" t="b">
@@ -1126,22 +1125,22 @@
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" s="1" t="s">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22">
         <v>7.7062821388244598E-3</v>
       </c>
-      <c r="K22" s="9" t="s">
+      <c r="K22" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="L22" s="15">
+      <c r="L22" s="14">
         <v>4.3047237396240199E-3</v>
       </c>
-      <c r="M22" s="22">
+      <c r="M22" s="21">
         <v>0.58616441011428799</v>
       </c>
       <c r="N22" t="b">
@@ -1150,22 +1149,22 @@
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23" s="1" t="s">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23">
         <v>4.3047237396240199E-3</v>
       </c>
-      <c r="K23" s="8" t="s">
+      <c r="K23" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L23" s="21">
+      <c r="L23" s="20">
         <v>6.5287613868713302E-3</v>
       </c>
-      <c r="M23" s="18">
+      <c r="M23" s="17">
         <v>5.3519296646118101E-3</v>
       </c>
       <c r="N23" t="b">
@@ -1174,22 +1173,22 @@
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="1" t="s">
+      <c r="A24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24">
         <v>0.58616441011428799</v>
       </c>
-      <c r="K24" s="9" t="s">
+      <c r="K24" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L24" s="15">
+      <c r="L24" s="14">
         <v>8.9594340324401795E-3</v>
       </c>
-      <c r="M24" s="22">
+      <c r="M24" s="21">
         <v>2.5084996223449698E-3</v>
       </c>
       <c r="N24" t="b">
@@ -1198,46 +1197,46 @@
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25" s="1" t="s">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25">
         <v>6.5287613868713302E-3</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" s="1" t="s">
+      <c r="A26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26">
         <v>5.3519296646118101E-3</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A27" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B27" s="1" t="s">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27">
         <v>8.9594340324401795E-3</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A28" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" s="1" t="s">
+      <c r="A28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" t="s">
         <v>10</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28">
         <v>2.5084996223449698E-3</v>
       </c>
     </row>

</xml_diff>